<commit_message>
Add autoincrement of test data
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yayie\SimpliLearn\selenium-java-maven\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453AFA06-BA63-42F4-961E-0D2887B9FFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B16191-C5F4-40F8-A24F-C5DAC1CB1C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="315" windowWidth="15720" windowHeight="12600" xr2:uid="{0B9F7A9C-42BA-4027-BF54-12895B2CCB0A}"/>
+    <workbookView xWindow="1185" yWindow="285" windowWidth="15720" windowHeight="12600" xr2:uid="{0B9F7A9C-42BA-4027-BF54-12895B2CCB0A}"/>
   </bookViews>
   <sheets>
     <sheet name="newaccountvalid" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="60">
   <si>
     <t>Mrs</t>
   </si>
@@ -214,10 +214,7 @@
     <t>Mr</t>
   </si>
   <si>
-    <t>emailemail205@email.com</t>
-  </si>
-  <si>
-    <t>emailemail206@email.com</t>
+    <t>emailemail@email.com</t>
   </si>
 </sst>
 </file>
@@ -682,7 +679,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>

</xml_diff>